<commit_message>
Add Login Page- Auth - Author
</commit_message>
<xml_diff>
--- a/work breakdown structure.xlsx
+++ b/work breakdown structure.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="37" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="45" uniqueCount="45">
   <si>
     <t>Account</t>
   </si>
@@ -212,6 +212,45 @@
 Name,
 Address,
 Descriptions</t>
+  </si>
+  <si>
+    <t>Order</t>
+  </si>
+  <si>
+    <t>OrderDetail</t>
+  </si>
+  <si>
+    <t>Products</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> BarCode: 
+   ProductName: 
+   OriginPrice: 
+   DisplayPrice
+   Category:
+   CreateAt:</t>
+  </si>
+  <si>
+    <t xml:space="preserve">OrderID
+BarCodeID
+Quantity,
+TotalPrice
+</t>
+  </si>
+  <si>
+    <t>Customer</t>
+  </si>
+  <si>
+    <t>Phone: unique
+fullName
+Address</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Staff
+CustomerPhone
+CreateAt
+TotalPayment
+</t>
   </si>
 </sst>
 </file>
@@ -3321,8 +3360,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:C23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+    <sheetView tabSelected="1" topLeftCell="A3" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="A8" sqref="A8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="33.75" x14ac:dyDescent="0.5"/>
@@ -3364,23 +3403,43 @@
       <c r="C3" s="15"/>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B4" s="15"/>
+      <c r="B4" s="16"/>
       <c r="C4" s="15"/>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B5" s="15"/>
+    <row r="5" spans="1:3" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A5" s="11" t="s">
+        <v>37</v>
+      </c>
+      <c r="B5" s="16" t="s">
+        <v>44</v>
+      </c>
       <c r="C5" s="15"/>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B6" s="15"/>
+    <row r="6" spans="1:3" ht="116.25" x14ac:dyDescent="0.35">
+      <c r="A6" s="11" t="s">
+        <v>38</v>
+      </c>
+      <c r="B6" s="16" t="s">
+        <v>41</v>
+      </c>
       <c r="C6" s="15"/>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B7" s="15"/>
+    <row r="7" spans="1:3" ht="69.75" x14ac:dyDescent="0.35">
+      <c r="A7" s="11" t="s">
+        <v>42</v>
+      </c>
+      <c r="B7" s="16" t="s">
+        <v>43</v>
+      </c>
       <c r="C7" s="15"/>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="B8" s="15"/>
+    <row r="8" spans="1:3" ht="186" x14ac:dyDescent="0.35">
+      <c r="A8" s="11" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>40</v>
+      </c>
       <c r="C8" s="15"/>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.5">
@@ -3445,5 +3504,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>